<commit_message>
Ajuste para la llamada de la descarga del Blockchain
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/bin/Documentos/Exportar/1.6.LSP_exp.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/bin/Documentos/Exportar/1.6.LSP_exp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JK\Desktop\EXCEL EXPORTAR LISTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Desktop\git-res\back-end\Web Dinamico 2\MRVMinem\Documentos\Exportar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A21A97-D7FC-484D-AC39-8A99A1A12195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18075" windowHeight="6885" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -25,22 +26,28 @@
     <definedName name="Lista_meses">Variables!$Z$20:$Z$31</definedName>
     <definedName name="Tabla_mes">Variables!$Z$20:$AA$31</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>MRV</author>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="134">
   <si>
     <t>1.6.</t>
   </si>
@@ -772,9 +779,6 @@
     </r>
   </si>
   <si>
-    <t>Inicio de Operaciones</t>
-  </si>
-  <si>
     <t>Potencia BAU (W)</t>
   </si>
   <si>
@@ -864,13 +868,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1684,10 +1688,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1805,7 +1809,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1813,94 +1817,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="17" fillId="12" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="16" fillId="13" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="17" fillId="13" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="12" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="17" fillId="12" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="13" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="17" fillId="13" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1915,9 +1847,6 @@
     <xf numFmtId="4" fontId="24" fillId="14" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1937,9 +1866,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="22" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1950,7 +1876,7 @@
     <xf numFmtId="3" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1958,6 +1884,81 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1997,7 +1998,13 @@
     <xdr:ext cx="3945701" cy="381985"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CuadroTexto 1"/>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2096,7 +2103,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CuadroTexto 2"/>
+        <xdr:cNvPr id="3" name="CuadroTexto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2191,7 +2204,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1" descr="Resultado de imagen para potencia de focos incandescentes"/>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Resultado de imagen para potencia de focos incandescentes">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2244,7 +2263,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="Resultado de imagen para lamparas equivalentes"/>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="Resultado de imagen para lamparas equivalentes">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2578,7 +2603,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2605,24 +2630,24 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="89"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="69"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="92"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="70"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="72"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="95"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -2723,7 +2748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2759,14 +2784,14 @@
       <c r="I2" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
@@ -2775,19 +2800,19 @@
       <c r="D5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="77" t="s">
+      <c r="K5" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="82" t="s">
+      <c r="M5" s="103"/>
+      <c r="N5" s="104"/>
+      <c r="O5" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="84"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="107"/>
     </row>
     <row r="6" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
@@ -2796,7 +2821,7 @@
       <c r="D6" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="78"/>
+      <c r="K6" s="101"/>
       <c r="L6" s="19" t="s">
         <v>55</v>
       </c>
@@ -2882,14 +2907,14 @@
       <c r="Q10" s="38"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="98"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
@@ -2965,180 +2990,166 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="88" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="88"/>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="88"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="88"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="91" t="s">
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="64"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="64"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="64"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="95" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="108" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="96" t="s">
+    <row r="5" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="73"/>
+      <c r="G5" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="96" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="98"/>
-      <c r="H5" s="99" t="s">
-        <v>119</v>
-      </c>
-      <c r="I5" s="95"/>
-    </row>
-    <row r="6" spans="2:9" ht="72" x14ac:dyDescent="0.25">
+      <c r="H5" s="108"/>
+    </row>
+    <row r="6" spans="2:8" ht="72" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40" t="s">
+      <c r="E6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="100"/>
-      <c r="H6" s="40" t="s">
+      <c r="F6" s="75"/>
+      <c r="G6" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="I6" s="101" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="102">
+      <c r="H6" s="76" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="77">
         <v>2017</v>
       </c>
-      <c r="C7" s="103">
-        <v>43524</v>
-      </c>
-      <c r="D7" s="104">
+      <c r="C7" s="78">
         <v>40</v>
       </c>
-      <c r="E7" s="104">
+      <c r="D7" s="78">
         <v>11</v>
       </c>
-      <c r="F7" s="104">
+      <c r="E7" s="78">
         <v>25000</v>
       </c>
-      <c r="G7" s="104">
-        <f>VLOOKUP(H7,Tabla_mes,2,FALSE)</f>
+      <c r="F7" s="78">
+        <f>VLOOKUP(G7,Tabla_mes,2,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="H7" s="104" t="s">
+      <c r="G7" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="I7" s="105">
-        <f>(((D7-E7)/(1-Factores!C11))*1/1000000*Factores!Q11*F7*Variables!$T$5)*G7/12</f>
+      <c r="H7" s="79">
+        <f>(((C7-D7)/(1-Factores!C11))*1/1000000*Factores!Q11*E7*Variables!$T$5)*F7/12</f>
         <v>810.17774663677119</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="102">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="77">
         <v>2018</v>
       </c>
-      <c r="C8" s="103">
-        <v>43647</v>
-      </c>
-      <c r="D8" s="104">
+      <c r="C8" s="78">
         <v>36</v>
       </c>
-      <c r="E8" s="104">
+      <c r="D8" s="78">
         <v>10</v>
       </c>
-      <c r="F8" s="104">
+      <c r="E8" s="78">
         <v>31000</v>
       </c>
-      <c r="G8" s="104">
-        <f>VLOOKUP(H8,Tabla_mes,2,FALSE)</f>
+      <c r="F8" s="78">
+        <f>VLOOKUP(G8,Tabla_mes,2,FALSE)</f>
         <v>10</v>
       </c>
-      <c r="H8" s="104" t="s">
+      <c r="G8" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="105">
-        <f>(((D8-E8)/(1-Factores!C12))*1/1000000*Factores!Q12*F8*Variables!$T$5)*G8/12</f>
+      <c r="H8" s="79">
+        <f>(((C8-D8)/(1-Factores!C12))*1/1000000*Factores!Q12*E8*Variables!$T$5)*F8/12</f>
         <v>818.81286995515711</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="106"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="110">
-        <f>SUM(I7:I8)</f>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="84">
+        <f>SUM(H7:H8)</f>
         <v>1628.9906165919283</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G8" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>Lista_meses</formula1>
     </dataValidation>
   </dataValidations>
@@ -3147,7 +3158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:PG45"/>
   <sheetViews>
     <sheetView topLeftCell="Q13" workbookViewId="0">
@@ -3223,18 +3234,18 @@
       <c r="B3" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
     </row>
     <row r="4" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="41" t="s">
@@ -3611,11 +3622,11 @@
       <c r="P19" s="41">
         <v>20</v>
       </c>
-      <c r="Z19" s="111" t="s">
+      <c r="Z19" s="85" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA19" s="86" t="s">
         <v>123</v>
-      </c>
-      <c r="AA19" s="112" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
@@ -3699,7 +3710,7 @@
         <v>90</v>
       </c>
       <c r="Z22" s="41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AA22" s="44">
         <v>9</v>
@@ -3728,7 +3739,7 @@
         <v>120</v>
       </c>
       <c r="Z23" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AA23" s="44">
         <v>8</v>
@@ -3757,7 +3768,7 @@
         <v>150</v>
       </c>
       <c r="Z24" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AA24" s="44">
         <v>7</v>
@@ -3771,7 +3782,7 @@
         <v>22</v>
       </c>
       <c r="Z25" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA25" s="44">
         <v>6</v>
@@ -3785,7 +3796,7 @@
         <v>32</v>
       </c>
       <c r="Z26" s="41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AA26" s="44">
         <v>5</v>
@@ -3799,7 +3810,7 @@
         <v>9</v>
       </c>
       <c r="Z27" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA27" s="44">
         <v>4</v>
@@ -3813,7 +3824,7 @@
         <v>11</v>
       </c>
       <c r="Z28" s="41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA28" s="44">
         <v>3</v>
@@ -3827,7 +3838,7 @@
         <v>15</v>
       </c>
       <c r="Z29" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA29" s="44">
         <v>2</v>
@@ -3841,7 +3852,7 @@
         <v>20</v>
       </c>
       <c r="Z30" s="41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA30" s="44">
         <v>1</v>
@@ -3855,7 +3866,7 @@
         <v>23</v>
       </c>
       <c r="Z31" s="41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA31" s="44">
         <v>0</v>
@@ -4419,8 +4430,8 @@
     <mergeCell ref="C3:L3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="R34" r:id="rId1"/>
-    <hyperlink ref="E32" r:id="rId2"/>
+    <hyperlink ref="R34" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E32" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
@@ -4428,7 +4439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -4790,35 +4801,35 @@
       <c r="Q24" s="55"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="O25" s="86" t="s">
+      <c r="O25" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="P25" s="86"/>
-      <c r="Q25" s="86"/>
+      <c r="P25" s="110"/>
+      <c r="Q25" s="110"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="O26" s="87"/>
-      <c r="P26" s="87"/>
-      <c r="Q26" s="87"/>
+      <c r="O26" s="111"/>
+      <c r="P26" s="111"/>
+      <c r="Q26" s="111"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="O27" s="87"/>
-      <c r="P27" s="87"/>
-      <c r="Q27" s="87"/>
+      <c r="O27" s="111"/>
+      <c r="P27" s="111"/>
+      <c r="Q27" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="O25:Q27"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1 Balance e Indicadores 2017.pdf"/>
-    <hyperlink ref="D10" r:id="rId2" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1  Balance e Indicadores 2016.pdf"/>
-    <hyperlink ref="D9" r:id="rId3" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1 Indicadores FINAL.pdf"/>
-    <hyperlink ref="D8" r:id="rId4" display="http://www.minem.gob.pe/minem/archivos/BALANCE E INDICADORES 2014.pdf"/>
-    <hyperlink ref="D7" r:id="rId5" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1  Balance y Principales Indicadores 2013.pdf"/>
-    <hyperlink ref="D6" r:id="rId6" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1  Balance y Principales Indicadores 2012.pdf"/>
-    <hyperlink ref="D5" r:id="rId7" display="http://www.minem.gob.pe/minem/archivos/Cap_1_  Balance y Principales Indicadores 2011.pdf"/>
-    <hyperlink ref="D4" r:id="rId8" display="http://www.minem.gob.pe/minem/archivos/Cap%C3%83%C2%ADtulo1_- Balance y Principales Indicadores El%C3%83%C2%A9ctricos 2010 (2).pdf"/>
+    <hyperlink ref="D11" r:id="rId1" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1 Balance e Indicadores 2017.pdf" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D10" r:id="rId2" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1  Balance e Indicadores 2016.pdf" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="D9" r:id="rId3" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1 Indicadores FINAL.pdf" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="D8" r:id="rId4" display="http://www.minem.gob.pe/minem/archivos/BALANCE E INDICADORES 2014.pdf" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="D7" r:id="rId5" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1  Balance y Principales Indicadores 2013.pdf" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="D6" r:id="rId6" display="http://www.minem.gob.pe/minem/archivos/Capitulo 1  Balance y Principales Indicadores 2012.pdf" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="D5" r:id="rId7" display="http://www.minem.gob.pe/minem/archivos/Cap_1_  Balance y Principales Indicadores 2011.pdf" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="D4" r:id="rId8" display="http://www.minem.gob.pe/minem/archivos/Cap%C3%83%C2%ADtulo1_- Balance y Principales Indicadores El%C3%83%C2%A9ctricos 2010 (2).pdf" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId9"/>

</xml_diff>